<commit_message>
Visualization Attempt 3 for December Meeting
</commit_message>
<xml_diff>
--- a/Data/master.xlsx
+++ b/Data/master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Projects\FoodHubs\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ta0jrg1\Documents\Projects\FoodHubs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3966C9F-B301-4B98-966E-00FD028D1325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94B144E-E1D8-4310-A549-0FA116A5C656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{7FA3B4B5-9D15-B84A-A7DB-0A68A34FD98B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7FA3B4B5-9D15-B84A-A7DB-0A68A34FD98B}"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="21" r:id="rId1"/>
@@ -177,7 +177,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2277" uniqueCount="983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="978">
   <si>
     <t>Hub</t>
   </si>
@@ -2990,27 +2990,18 @@
     <t>#007F00</t>
   </si>
   <si>
-    <t>Wholesale Focus</t>
-  </si>
-  <si>
     <t>narrow</t>
   </si>
   <si>
     <t>#7F007F</t>
   </si>
   <si>
-    <t>Mostly Indstitutionally</t>
-  </si>
-  <si>
     <t>full-spectrum</t>
   </si>
   <si>
     <t>#197319</t>
   </si>
   <si>
-    <t>Diverse</t>
-  </si>
-  <si>
     <t>specialized</t>
   </si>
   <si>
@@ -3029,12 +3020,6 @@
     <t>#734619</t>
   </si>
   <si>
-    <t>Mostly Institutional</t>
-  </si>
-  <si>
-    <t>Instiutional Focus</t>
-  </si>
-  <si>
     <t>#7F4633</t>
   </si>
   <si>
@@ -3062,9 +3047,6 @@
     <t>Ranked_Social</t>
   </si>
   <si>
-    <t>Sale_Point</t>
-  </si>
-  <si>
     <t>Instructions</t>
   </si>
   <si>
@@ -3101,9 +3083,6 @@
     <t>Hub_Name</t>
   </si>
   <si>
-    <t>Direct-to-Consumer</t>
-  </si>
-  <si>
     <t>Global_Social</t>
   </si>
   <si>
@@ -3126,6 +3105,12 @@
   </si>
   <si>
     <t>BM_Scale</t>
+  </si>
+  <si>
+    <t>Business_Model</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -3673,228 +3658,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D66AB6-4D2C-4516-876E-80F25D4C8C14}">
-  <dimension ref="A1:AW13"/>
+  <dimension ref="A1:AX13"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AB5" sqref="AB5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="262.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="261" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>889</v>
       </c>
       <c r="B1" t="s">
+        <v>967</v>
+      </c>
+      <c r="C1" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1" t="s">
+        <v>966</v>
+      </c>
+      <c r="E1" t="s">
+        <v>965</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>976</v>
+      </c>
+      <c r="G1" t="s">
+        <v>964</v>
+      </c>
+      <c r="H1" t="s">
+        <v>963</v>
+      </c>
+      <c r="I1" t="s">
+        <v>962</v>
+      </c>
+      <c r="J1" t="s">
+        <v>961</v>
+      </c>
+      <c r="K1" t="s">
+        <v>960</v>
+      </c>
+      <c r="L1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M1" t="s">
+        <v>194</v>
+      </c>
+      <c r="N1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O1" t="s">
+        <v>196</v>
+      </c>
+      <c r="P1" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>959</v>
+      </c>
+      <c r="R1" t="s">
+        <v>958</v>
+      </c>
+      <c r="S1" t="s">
+        <v>957</v>
+      </c>
+      <c r="T1" t="s">
+        <v>956</v>
+      </c>
+      <c r="U1" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z1" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC1" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>972</v>
+      </c>
+      <c r="AH1" t="s">
         <v>973</v>
       </c>
-      <c r="C1" t="s">
-        <v>972</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="AI1" t="s">
+        <v>974</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>968</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>969</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>970</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>955</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>954</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>953</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>952</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>951</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>950</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>949</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>948</v>
+      </c>
+      <c r="AX1" t="s">
         <v>971</v>
       </c>
-      <c r="E1" t="s">
-        <v>970</v>
-      </c>
-      <c r="F1" t="s">
-        <v>969</v>
-      </c>
-      <c r="G1" t="s">
-        <v>968</v>
-      </c>
-      <c r="H1" t="s">
-        <v>967</v>
-      </c>
-      <c r="I1" t="s">
-        <v>966</v>
-      </c>
-      <c r="J1" t="s">
-        <v>199</v>
-      </c>
-      <c r="K1" t="s">
-        <v>194</v>
-      </c>
-      <c r="L1" t="s">
-        <v>195</v>
-      </c>
-      <c r="M1" t="s">
-        <v>196</v>
-      </c>
-      <c r="N1" t="s">
-        <v>198</v>
-      </c>
-      <c r="O1" t="s">
-        <v>965</v>
-      </c>
-      <c r="P1" t="s">
-        <v>964</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>963</v>
-      </c>
-      <c r="R1" t="s">
-        <v>962</v>
-      </c>
-      <c r="S1" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" t="s">
-        <v>961</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="V1" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="W1" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="X1" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y1" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z1" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA1" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB1" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC1" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD1" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE1" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>979</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>980</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>981</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>975</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>976</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>977</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>960</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>959</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>958</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>957</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>956</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>955</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>954</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>953</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>871</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>935</v>
       </c>
-      <c r="E2" t="s">
-        <v>201</v>
-      </c>
       <c r="F2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G2" t="s">
         <v>201</v>
@@ -3902,11 +3891,11 @@
       <c r="H2" t="s">
         <v>201</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
+      <c r="I2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J2" t="s">
+        <v>201</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3923,23 +3912,23 @@
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2" t="s">
-        <v>201</v>
+      <c r="P2">
+        <v>0</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S2">
         <v>100</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2" t="s">
-        <v>974</v>
-      </c>
-      <c r="U2" t="s">
-        <v>201</v>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
       </c>
       <c r="V2" t="s">
         <v>201</v>
@@ -3980,67 +3969,70 @@
       <c r="AH2" t="s">
         <v>201</v>
       </c>
-      <c r="AI2">
-        <v>3</v>
+      <c r="AI2" t="s">
+        <v>201</v>
       </c>
       <c r="AJ2">
         <v>3</v>
       </c>
       <c r="AK2">
+        <v>3</v>
+      </c>
+      <c r="AL2">
         <v>2</v>
       </c>
-      <c r="AL2">
+      <c r="AM2">
         <v>3</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>2</v>
       </c>
-      <c r="AN2">
-        <v>1</v>
-      </c>
       <c r="AO2">
+        <v>1</v>
+      </c>
+      <c r="AP2">
         <v>177.06984362075525</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>502.86279698478472</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <v>110.02609983990698</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>312.46445569423616</v>
       </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
       <c r="AT2">
         <v>0</v>
       </c>
       <c r="AU2">
         <v>0</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>872</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
-        <v>46</v>
+      <c r="C3">
+        <v>30</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>205</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -4058,37 +4050,37 @@
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" t="s">
         <v>934</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>10</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>90</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3" t="s">
-        <v>951</v>
-      </c>
       <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
         <v>2</v>
-      </c>
-      <c r="V3">
-        <v>3</v>
       </c>
       <c r="W3">
         <v>3</v>
@@ -4097,16 +4089,16 @@
         <v>3</v>
       </c>
       <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
         <v>2</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>3</v>
       </c>
-      <c r="AA3">
+      <c r="AB3">
         <v>2</v>
-      </c>
-      <c r="AB3">
-        <v>3</v>
       </c>
       <c r="AC3">
         <v>3</v>
@@ -4115,129 +4107,132 @@
         <v>3</v>
       </c>
       <c r="AE3">
+        <v>3</v>
+      </c>
+      <c r="AF3">
         <v>2</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>2.6</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>2.75</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>2.5</v>
-      </c>
-      <c r="AI3">
-        <v>3</v>
       </c>
       <c r="AJ3">
         <v>3</v>
       </c>
       <c r="AK3">
+        <v>3</v>
+      </c>
+      <c r="AL3">
         <v>2</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>3</v>
       </c>
-      <c r="AM3">
+      <c r="AN3">
         <v>2</v>
       </c>
-      <c r="AN3">
-        <v>1</v>
-      </c>
       <c r="AO3">
+        <v>1</v>
+      </c>
+      <c r="AP3">
         <v>66.730648916437048</v>
       </c>
-      <c r="AP3">
+      <c r="AQ3">
         <v>180.79488361545049</v>
       </c>
-      <c r="AQ3">
+      <c r="AR3">
         <v>41.464502875977445</v>
       </c>
-      <c r="AR3">
+      <c r="AS3">
         <v>112.34073238254251</v>
       </c>
-      <c r="AS3">
+      <c r="AT3">
         <v>0.5</v>
       </c>
-      <c r="AT3">
+      <c r="AU3">
         <v>0.3</v>
       </c>
-      <c r="AU3">
+      <c r="AV3">
         <v>0.2</v>
       </c>
-      <c r="AV3" t="s">
-        <v>952</v>
-      </c>
       <c r="AW3" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+        <v>947</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>873</v>
       </c>
       <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>360</v>
+      </c>
+      <c r="D4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>165</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="F4" t="s">
+        <v>59</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" t="s">
-        <v>938</v>
+      <c r="P4">
+        <v>0</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
-      <c r="R4">
+      <c r="R4" t="s">
+        <v>937</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
         <v>100</v>
       </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4" t="s">
-        <v>951</v>
-      </c>
       <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
         <v>2</v>
-      </c>
-      <c r="V4">
-        <v>3</v>
       </c>
       <c r="W4">
         <v>3</v>
@@ -4252,93 +4247,96 @@
         <v>3</v>
       </c>
       <c r="AA4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB4">
         <v>2</v>
       </c>
       <c r="AC4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD4">
         <v>3</v>
       </c>
       <c r="AE4">
+        <v>3</v>
+      </c>
+      <c r="AF4">
         <v>2</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>2.8</v>
-      </c>
-      <c r="AG4">
-        <v>2.5</v>
       </c>
       <c r="AH4">
         <v>2.5</v>
       </c>
       <c r="AI4">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="AJ4">
         <v>2</v>
       </c>
       <c r="AK4">
+        <v>2</v>
+      </c>
+      <c r="AL4">
         <v>3</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>2</v>
       </c>
-      <c r="AM4">
-        <v>1</v>
-      </c>
       <c r="AN4">
+        <v>1</v>
+      </c>
+      <c r="AO4">
         <v>3</v>
       </c>
-      <c r="AO4">
+      <c r="AP4">
         <v>54.000686345069504</v>
       </c>
-      <c r="AP4">
+      <c r="AQ4">
         <v>107.42790056424694</v>
       </c>
-      <c r="AQ4">
+      <c r="AR4">
         <v>33.554470855870157</v>
       </c>
-      <c r="AR4">
+      <c r="AS4">
         <v>66.752602653159883</v>
       </c>
-      <c r="AS4">
-        <v>1</v>
-      </c>
       <c r="AT4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU4">
         <v>0</v>
       </c>
-      <c r="AV4" t="s">
-        <v>948</v>
+      <c r="AV4">
+        <v>0</v>
       </c>
       <c r="AW4" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+        <v>945</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>874</v>
       </c>
       <c r="B5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s">
-        <v>46</v>
+      <c r="C5">
+        <v>330</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" t="s">
+        <v>205</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -4353,7 +4351,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -4367,42 +4365,42 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" t="s">
-        <v>941</v>
+      <c r="P5">
+        <v>0</v>
       </c>
       <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>939</v>
+      </c>
+      <c r="S5">
         <v>33</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>64</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>3</v>
       </c>
-      <c r="T5" t="s">
-        <v>950</v>
-      </c>
-      <c r="U5">
+      <c r="V5">
         <v>2</v>
-      </c>
-      <c r="V5">
-        <v>3</v>
       </c>
       <c r="W5">
         <v>3</v>
       </c>
       <c r="X5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y5">
         <v>1</v>
       </c>
       <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
         <v>2</v>
       </c>
-      <c r="AA5">
-        <v>1</v>
-      </c>
       <c r="AB5">
         <v>1</v>
       </c>
@@ -4410,22 +4408,22 @@
         <v>1</v>
       </c>
       <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
         <v>2</v>
       </c>
-      <c r="AE5">
-        <v>1</v>
-      </c>
       <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
         <v>2</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>1.25</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>1.5</v>
-      </c>
-      <c r="AI5">
-        <v>2</v>
       </c>
       <c r="AJ5">
         <v>2</v>
@@ -4434,60 +4432,63 @@
         <v>2</v>
       </c>
       <c r="AL5">
+        <v>2</v>
+      </c>
+      <c r="AM5">
         <v>3</v>
       </c>
-      <c r="AM5">
+      <c r="AN5">
         <v>2</v>
       </c>
-      <c r="AN5">
-        <v>1</v>
-      </c>
       <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
         <v>59.07183056002777</v>
       </c>
-      <c r="AP5">
+      <c r="AQ5">
         <v>62.670818674705536</v>
       </c>
-      <c r="AQ5">
+      <c r="AR5">
         <v>36.705533782726235</v>
       </c>
-      <c r="AR5">
+      <c r="AS5">
         <v>38.941841318391553</v>
-      </c>
-      <c r="AS5">
-        <v>0.45</v>
       </c>
       <c r="AT5">
         <v>0.45</v>
       </c>
       <c r="AU5">
+        <v>0.45</v>
+      </c>
+      <c r="AV5">
         <v>0.1</v>
       </c>
-      <c r="AV5" t="s">
-        <v>949</v>
-      </c>
       <c r="AW5" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+        <v>946</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>875</v>
       </c>
       <c r="B6" t="s">
         <v>79</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6" t="s">
         <v>80</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>935</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
+      <c r="F6" t="s">
+        <v>203</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -4502,40 +4503,40 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6" t="s">
-        <v>941</v>
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
       </c>
       <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>939</v>
+      </c>
+      <c r="S6">
         <v>80</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>20</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6" t="s">
-        <v>974</v>
-      </c>
       <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
         <v>2</v>
-      </c>
-      <c r="V6">
-        <v>3</v>
       </c>
       <c r="W6">
         <v>3</v>
@@ -4565,90 +4566,93 @@
         <v>3</v>
       </c>
       <c r="AF6">
+        <v>3</v>
+      </c>
+      <c r="AG6">
         <v>2.8</v>
-      </c>
-      <c r="AG6">
-        <v>3</v>
       </c>
       <c r="AH6">
         <v>3</v>
       </c>
       <c r="AI6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ6">
         <v>2</v>
       </c>
       <c r="AK6">
+        <v>2</v>
+      </c>
+      <c r="AL6">
         <v>3</v>
       </c>
-      <c r="AL6">
-        <v>1</v>
-      </c>
       <c r="AM6">
+        <v>1</v>
+      </c>
+      <c r="AN6">
         <v>2</v>
       </c>
-      <c r="AN6">
+      <c r="AO6">
         <v>3</v>
       </c>
-      <c r="AO6">
+      <c r="AP6">
         <v>61.132335382406808</v>
       </c>
-      <c r="AP6">
+      <c r="AQ6">
         <v>510.85624675116685</v>
       </c>
-      <c r="AQ6">
+      <c r="AR6">
         <v>37.985872120818676</v>
       </c>
-      <c r="AR6">
+      <c r="AS6">
         <v>317.43135510566225</v>
       </c>
-      <c r="AS6">
-        <v>1</v>
-      </c>
       <c r="AT6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU6">
         <v>0</v>
       </c>
-      <c r="AV6" t="s">
-        <v>948</v>
+      <c r="AV6">
+        <v>0</v>
       </c>
       <c r="AW6" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+        <v>945</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>876</v>
       </c>
       <c r="B7" t="s">
         <v>89</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7">
+        <v>270</v>
+      </c>
+      <c r="D7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>935</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+      <c r="F7" t="s">
+        <v>207</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -4663,25 +4667,25 @@
         <v>1</v>
       </c>
       <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7" t="s">
-        <v>941</v>
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
-      <c r="R7">
-        <v>0</v>
+      <c r="R7" t="s">
+        <v>939</v>
       </c>
       <c r="S7">
         <v>0</v>
       </c>
-      <c r="T7" t="s">
-        <v>201</v>
-      </c>
-      <c r="U7" t="s">
-        <v>201</v>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
       </c>
       <c r="V7" t="s">
         <v>201</v>
@@ -4722,26 +4726,26 @@
       <c r="AH7" t="s">
         <v>201</v>
       </c>
-      <c r="AI7">
-        <v>2</v>
+      <c r="AI7" t="s">
+        <v>201</v>
       </c>
       <c r="AJ7">
         <v>2</v>
       </c>
       <c r="AK7">
+        <v>2</v>
+      </c>
+      <c r="AL7">
         <v>3</v>
       </c>
-      <c r="AL7">
+      <c r="AM7">
         <v>2</v>
       </c>
-      <c r="AM7">
-        <v>1</v>
-      </c>
       <c r="AN7">
+        <v>1</v>
+      </c>
+      <c r="AO7">
         <v>3</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>201</v>
       </c>
       <c r="AP7" t="s">
         <v>201</v>
@@ -4752,49 +4756,52 @@
       <c r="AR7" t="s">
         <v>201</v>
       </c>
-      <c r="AS7">
+      <c r="AS7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT7">
         <v>0.1</v>
       </c>
-      <c r="AT7">
-        <v>0</v>
-      </c>
       <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
         <v>0.9</v>
       </c>
-      <c r="AV7" t="s">
-        <v>947</v>
-      </c>
       <c r="AW7" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+        <v>944</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>877</v>
       </c>
       <c r="B8" t="s">
         <v>98</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8">
+        <v>240</v>
+      </c>
+      <c r="D8" t="s">
         <v>57</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>165</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+      <c r="F8" t="s">
+        <v>207</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -4812,28 +4819,28 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8" t="s">
-        <v>938</v>
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
       </c>
       <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>937</v>
+      </c>
+      <c r="S8">
         <v>80</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>15</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>5</v>
       </c>
-      <c r="T8" t="s">
-        <v>974</v>
-      </c>
-      <c r="U8">
+      <c r="V8">
         <v>2</v>
-      </c>
-      <c r="V8">
-        <v>3</v>
       </c>
       <c r="W8">
         <v>3</v>
@@ -4845,7 +4852,7 @@
         <v>3</v>
       </c>
       <c r="Z8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA8">
         <v>2</v>
@@ -4854,105 +4861,108 @@
         <v>2</v>
       </c>
       <c r="AC8">
+        <v>2</v>
+      </c>
+      <c r="AD8">
         <v>3</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>2</v>
       </c>
-      <c r="AE8">
-        <v>1</v>
-      </c>
       <c r="AF8">
+        <v>1</v>
+      </c>
+      <c r="AG8">
         <v>2.8</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>2.25</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>1.5</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <v>2</v>
       </c>
-      <c r="AJ8">
-        <v>1</v>
-      </c>
       <c r="AK8">
+        <v>1</v>
+      </c>
+      <c r="AL8">
         <v>3</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>2</v>
       </c>
-      <c r="AM8">
-        <v>1</v>
-      </c>
       <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
         <v>3</v>
       </c>
-      <c r="AO8">
+      <c r="AP8">
         <v>42.020373634883299</v>
       </c>
-      <c r="AP8">
+      <c r="AQ8">
         <v>244.99066061451242</v>
       </c>
-      <c r="AQ8">
+      <c r="AR8">
         <v>26.110249663765671</v>
       </c>
-      <c r="AR8">
+      <c r="AS8">
         <v>152.23013887305163</v>
       </c>
-      <c r="AS8">
+      <c r="AT8">
         <v>0.9</v>
       </c>
-      <c r="AT8">
+      <c r="AU8">
         <v>0.1</v>
       </c>
-      <c r="AU8">
-        <v>0</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>946</v>
+      <c r="AV8">
+        <v>0</v>
       </c>
       <c r="AW8" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+        <v>943</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>878</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
-        <v>46</v>
+      <c r="C9">
+        <v>210</v>
       </c>
       <c r="D9" t="s">
         <v>46</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>207</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -4963,23 +4973,23 @@
       <c r="O9">
         <v>1</v>
       </c>
-      <c r="P9" t="s">
-        <v>941</v>
+      <c r="P9">
+        <v>1</v>
       </c>
       <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>939</v>
+      </c>
+      <c r="S9">
         <v>90</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>10</v>
       </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9" t="s">
-        <v>974</v>
-      </c>
       <c r="U9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V9">
         <v>3</v>
@@ -4988,7 +4998,7 @@
         <v>3</v>
       </c>
       <c r="X9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y9">
         <v>2</v>
@@ -5012,84 +5022,87 @@
         <v>2</v>
       </c>
       <c r="AF9">
+        <v>2</v>
+      </c>
+      <c r="AG9">
         <v>2.6</v>
-      </c>
-      <c r="AG9">
-        <v>2</v>
       </c>
       <c r="AH9">
         <v>2</v>
       </c>
       <c r="AI9">
+        <v>2</v>
+      </c>
+      <c r="AJ9">
         <v>2.5</v>
-      </c>
-      <c r="AJ9">
-        <v>3</v>
       </c>
       <c r="AK9">
         <v>3</v>
       </c>
       <c r="AL9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AM9">
+        <v>1</v>
+      </c>
+      <c r="AN9">
         <v>2</v>
       </c>
-      <c r="AN9">
+      <c r="AO9">
         <v>3</v>
       </c>
-      <c r="AO9">
+      <c r="AP9">
         <v>69.284801167278431</v>
       </c>
-      <c r="AP9">
+      <c r="AQ9">
         <v>217.13337565699663</v>
       </c>
-      <c r="AQ9">
+      <c r="AR9">
         <v>43.051579505238429</v>
       </c>
-      <c r="AR9">
+      <c r="AS9">
         <v>134.9204245065049</v>
-      </c>
-      <c r="AS9">
-        <v>0.5</v>
       </c>
       <c r="AT9">
         <v>0.5</v>
       </c>
       <c r="AU9">
-        <v>0</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>945</v>
+        <v>0.5</v>
+      </c>
+      <c r="AV9">
+        <v>0</v>
       </c>
       <c r="AW9" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+        <v>942</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>879</v>
       </c>
       <c r="B10" t="s">
         <v>119</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10">
+        <v>180</v>
+      </c>
+      <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>935</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
+      <c r="F10" t="s">
+        <v>149</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -5112,23 +5125,23 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10" t="s">
-        <v>944</v>
+      <c r="P10">
+        <v>0</v>
       </c>
       <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10" t="s">
+        <v>941</v>
+      </c>
+      <c r="S10">
         <v>34</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>33</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>33</v>
-      </c>
-      <c r="T10" t="s">
-        <v>943</v>
-      </c>
-      <c r="U10" t="s">
-        <v>201</v>
       </c>
       <c r="V10" t="s">
         <v>201</v>
@@ -5169,26 +5182,26 @@
       <c r="AH10" t="s">
         <v>201</v>
       </c>
-      <c r="AI10">
-        <v>3</v>
+      <c r="AI10" t="s">
+        <v>201</v>
       </c>
       <c r="AJ10">
         <v>3</v>
       </c>
       <c r="AK10">
+        <v>3</v>
+      </c>
+      <c r="AL10">
         <v>2</v>
       </c>
-      <c r="AL10">
+      <c r="AM10">
         <v>3</v>
       </c>
-      <c r="AM10">
+      <c r="AN10">
         <v>2</v>
       </c>
-      <c r="AN10">
-        <v>1</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>201</v>
+      <c r="AO10">
+        <v>1</v>
       </c>
       <c r="AP10" t="s">
         <v>201</v>
@@ -5199,46 +5212,49 @@
       <c r="AR10" t="s">
         <v>201</v>
       </c>
-      <c r="AS10">
+      <c r="AS10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT10">
         <v>0.1</v>
-      </c>
-      <c r="AT10">
-        <v>0.45</v>
       </c>
       <c r="AU10">
         <v>0.45</v>
       </c>
-      <c r="AV10" t="s">
-        <v>942</v>
+      <c r="AV10">
+        <v>0.45</v>
       </c>
       <c r="AW10" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+        <v>940</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>880</v>
       </c>
       <c r="B11" t="s">
         <v>129</v>
       </c>
-      <c r="C11" t="s">
-        <v>46</v>
+      <c r="C11">
+        <v>150</v>
       </c>
       <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" t="s">
+        <v>201</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -5250,7 +5266,7 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <v>1</v>
@@ -5259,28 +5275,28 @@
         <v>1</v>
       </c>
       <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>941</v>
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
       </c>
       <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11" t="s">
+        <v>939</v>
+      </c>
+      <c r="S11">
         <v>25</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>47</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>28</v>
       </c>
-      <c r="T11" t="s">
-        <v>940</v>
-      </c>
-      <c r="U11">
-        <v>1</v>
-      </c>
       <c r="V11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="W11">
         <v>3</v>
@@ -5298,25 +5314,25 @@
         <v>3</v>
       </c>
       <c r="AB11">
+        <v>3</v>
+      </c>
+      <c r="AC11">
         <v>2</v>
       </c>
-      <c r="AC11">
+      <c r="AD11">
         <v>3</v>
-      </c>
-      <c r="AD11">
-        <v>2</v>
       </c>
       <c r="AE11">
         <v>2</v>
       </c>
       <c r="AF11">
+        <v>2</v>
+      </c>
+      <c r="AG11">
         <v>2.6</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>2.75</v>
-      </c>
-      <c r="AH11">
-        <v>2</v>
       </c>
       <c r="AI11">
         <v>2</v>
@@ -5325,66 +5341,69 @@
         <v>2</v>
       </c>
       <c r="AK11">
+        <v>2</v>
+      </c>
+      <c r="AL11">
         <v>3</v>
       </c>
-      <c r="AL11">
+      <c r="AM11">
         <v>2</v>
       </c>
-      <c r="AM11">
-        <v>1</v>
-      </c>
       <c r="AN11">
+        <v>1</v>
+      </c>
+      <c r="AO11">
         <v>3</v>
       </c>
-      <c r="AO11">
+      <c r="AP11">
         <v>49.269501231495838</v>
       </c>
-      <c r="AP11">
+      <c r="AQ11">
         <v>219.39060746351947</v>
       </c>
-      <c r="AQ11">
+      <c r="AR11">
         <v>30.614648721153365</v>
       </c>
-      <c r="AR11">
+      <c r="AS11">
         <v>136.32300332528004</v>
       </c>
-      <c r="AS11">
+      <c r="AT11">
         <v>0.5</v>
       </c>
-      <c r="AT11">
-        <v>0</v>
-      </c>
       <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
         <v>0.5</v>
       </c>
-      <c r="AV11" t="s">
-        <v>939</v>
-      </c>
       <c r="AW11" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+        <v>938</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>881</v>
       </c>
       <c r="B12" t="s">
         <v>138</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>120</v>
+      </c>
+      <c r="D12" t="s">
         <v>139</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>165</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" t="s">
+        <v>59</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -5396,7 +5415,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>0</v>
@@ -5408,25 +5427,25 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
-      </c>
-      <c r="P12" t="s">
-        <v>938</v>
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="R12">
+      <c r="R12" t="s">
+        <v>937</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
         <v>10</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>90</v>
-      </c>
-      <c r="T12" t="s">
-        <v>937</v>
-      </c>
-      <c r="U12" t="s">
-        <v>201</v>
       </c>
       <c r="V12" t="s">
         <v>201</v>
@@ -5467,79 +5486,82 @@
       <c r="AH12" t="s">
         <v>201</v>
       </c>
-      <c r="AI12">
-        <v>2</v>
+      <c r="AI12" t="s">
+        <v>201</v>
       </c>
       <c r="AJ12">
         <v>2</v>
       </c>
       <c r="AK12">
+        <v>2</v>
+      </c>
+      <c r="AL12">
         <v>3</v>
       </c>
-      <c r="AL12">
+      <c r="AM12">
         <v>2</v>
       </c>
-      <c r="AM12">
-        <v>1</v>
-      </c>
       <c r="AN12">
+        <v>1</v>
+      </c>
+      <c r="AO12">
         <v>3</v>
       </c>
-      <c r="AO12">
+      <c r="AP12">
         <v>102.89933989204253</v>
       </c>
-      <c r="AP12">
+      <c r="AQ12">
         <v>195.67903527505888</v>
       </c>
-      <c r="AQ12">
+      <c r="AR12">
         <v>63.938685509153132</v>
       </c>
-      <c r="AR12">
+      <c r="AS12">
         <v>121.58931544471467</v>
       </c>
-      <c r="AS12">
-        <v>0</v>
-      </c>
       <c r="AT12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AU12">
         <v>0.5</v>
       </c>
-      <c r="AV12" t="s">
-        <v>936</v>
+      <c r="AV12">
+        <v>0.5</v>
       </c>
       <c r="AW12" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX12" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>882</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13">
+        <v>90</v>
+      </c>
+      <c r="D13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>935</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
+      <c r="F13" t="s">
+        <v>149</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -5548,34 +5570,34 @@
         <v>1</v>
       </c>
       <c r="L13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
         <v>934</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>80</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>20</v>
       </c>
-      <c r="S13">
-        <v>0</v>
-      </c>
-      <c r="T13" t="s">
-        <v>974</v>
-      </c>
       <c r="U13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V13">
         <v>3</v>
@@ -5584,40 +5606,40 @@
         <v>3</v>
       </c>
       <c r="X13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y13">
         <v>1</v>
       </c>
       <c r="Z13">
+        <v>1</v>
+      </c>
+      <c r="AA13">
         <v>3</v>
       </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
       <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
         <v>2</v>
       </c>
-      <c r="AC13">
+      <c r="AD13">
         <v>3</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>2</v>
       </c>
-      <c r="AE13">
-        <v>1</v>
-      </c>
       <c r="AF13">
+        <v>1</v>
+      </c>
+      <c r="AG13">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AG13">
+      <c r="AH13">
         <v>2.6666666666666665</v>
       </c>
-      <c r="AH13">
+      <c r="AI13">
         <v>1.5</v>
-      </c>
-      <c r="AI13">
-        <v>2</v>
       </c>
       <c r="AJ13">
         <v>2</v>
@@ -5629,13 +5651,13 @@
         <v>2</v>
       </c>
       <c r="AM13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN13">
+        <v>1</v>
+      </c>
+      <c r="AO13">
         <v>3</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>201</v>
       </c>
       <c r="AP13" t="s">
         <v>201</v>
@@ -5646,19 +5668,22 @@
       <c r="AR13" t="s">
         <v>201</v>
       </c>
-      <c r="AS13">
+      <c r="AS13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT13">
         <v>0.5</v>
       </c>
-      <c r="AT13">
+      <c r="AU13">
         <v>0.45</v>
       </c>
-      <c r="AU13">
+      <c r="AV13">
         <v>0.05</v>
       </c>
-      <c r="AV13" t="s">
+      <c r="AW13" t="s">
         <v>933</v>
       </c>
-      <c r="AW13" t="s">
+      <c r="AX13" t="s">
         <v>933</v>
       </c>
     </row>
@@ -15349,7 +15374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B59C92-0A90-4A23-B4F3-52F301A8F7BD}">
   <dimension ref="A1:AL37"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
@@ -16871,8 +16896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC08EB3-8594-4879-B4C1-F4C5F04945E6}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16906,7 +16931,7 @@
         <v>173</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>982</v>
+        <v>975</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Completed Clock Function and it seems to work.
</commit_message>
<xml_diff>
--- a/Data/master.xlsx
+++ b/Data/master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ta0jrg1\Documents\Projects\FoodHubs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9325BCB-0B7F-46FB-8FD7-49BA4F5CC0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455D3EE8-7A45-4E30-B1A3-A1CA8BD6E385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7FA3B4B5-9D15-B84A-A7DB-0A68A34FD98B}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{7FA3B4B5-9D15-B84A-A7DB-0A68A34FD98B}"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="21" r:id="rId1"/>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2302" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2317" uniqueCount="979">
   <si>
     <t>Hub</t>
   </si>
@@ -3039,18 +3039,6 @@
     <t>Aver_Dist_KM</t>
   </si>
   <si>
-    <t>Ranked_Econ</t>
-  </si>
-  <si>
-    <t>Ranked_Envrio</t>
-  </si>
-  <si>
-    <t>Ranked_Social</t>
-  </si>
-  <si>
-    <t>Instructions</t>
-  </si>
-  <si>
     <t>Households</t>
   </si>
   <si>
@@ -3096,15 +3084,6 @@
     <t>Color_Text</t>
   </si>
   <si>
-    <t>Local_Economic</t>
-  </si>
-  <si>
-    <t>Local_Social</t>
-  </si>
-  <si>
-    <t>Local_Environmental</t>
-  </si>
-  <si>
     <t>BM_Scale</t>
   </si>
   <si>
@@ -3117,10 +3096,25 @@
     <t>show</t>
   </si>
   <si>
-    <t>size_scale</t>
-  </si>
-  <si>
     <t>Gross_Revenue</t>
+  </si>
+  <si>
+    <t>size_scale_rev</t>
+  </si>
+  <si>
+    <t>size_scale_emp</t>
+  </si>
+  <si>
+    <t>Economic_Avg</t>
+  </si>
+  <si>
+    <t>Social_Avg</t>
+  </si>
+  <si>
+    <t>Environmental_Avg</t>
+  </si>
+  <si>
+    <t>Institutions</t>
   </si>
 </sst>
 </file>
@@ -3133,7 +3127,7 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -3348,13 +3342,13 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3670,10 +3664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D66AB6-4D2C-4516-876E-80F25D4C8C14}">
-  <dimension ref="A1:AX13"/>
+  <dimension ref="A1:AY13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AX14" sqref="AX14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3713,52 +3707,52 @@
     <col min="36" max="36" width="11.875" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="17.5" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="15" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="261" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" ht="261" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>889</v>
       </c>
       <c r="B1" t="s">
-        <v>967</v>
+        <v>963</v>
       </c>
       <c r="C1" t="s">
-        <v>977</v>
+        <v>970</v>
       </c>
       <c r="D1" t="s">
-        <v>966</v>
+        <v>962</v>
       </c>
       <c r="E1" t="s">
-        <v>965</v>
+        <v>961</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>976</v>
+        <v>969</v>
       </c>
       <c r="G1" t="s">
-        <v>964</v>
+        <v>960</v>
       </c>
       <c r="H1" t="s">
-        <v>963</v>
+        <v>959</v>
       </c>
       <c r="I1" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="J1" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="K1" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="L1" t="s">
         <v>199</v>
@@ -3776,16 +3770,16 @@
         <v>198</v>
       </c>
       <c r="Q1" t="s">
-        <v>959</v>
+        <v>955</v>
       </c>
       <c r="R1" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="S1" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="T1" t="s">
-        <v>956</v>
+        <v>978</v>
       </c>
       <c r="U1" t="s">
         <v>59</v>
@@ -3824,61 +3818,64 @@
         <v>9</v>
       </c>
       <c r="AG1" t="s">
+        <v>975</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>976</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>977</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>964</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>965</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>966</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>952</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>951</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>950</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>949</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>185</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>948</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>967</v>
+      </c>
+      <c r="AV1" s="2" t="s">
         <v>972</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AW1" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>973</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>974</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>968</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>969</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>970</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>955</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>954</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>953</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>952</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>951</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>950</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>949</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>185</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>186</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>948</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>871</v>
       </c>
@@ -3994,40 +3991,37 @@
         <v>2</v>
       </c>
       <c r="AM2">
-        <v>3</v>
+        <v>177.06984362075525</v>
       </c>
       <c r="AN2">
-        <v>2</v>
+        <v>502.86279698478472</v>
       </c>
       <c r="AO2">
-        <v>1</v>
+        <v>110.02609983990698</v>
       </c>
       <c r="AP2">
-        <v>177.06984362075525</v>
+        <v>312.46445569423616</v>
       </c>
       <c r="AQ2">
-        <v>502.86279698478472</v>
+        <v>0</v>
       </c>
       <c r="AR2">
-        <v>110.02609983990698</v>
+        <v>0</v>
       </c>
       <c r="AS2">
-        <v>312.46445569423616</v>
-      </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
-      <c r="AU2">
-        <v>0</v>
-      </c>
-      <c r="AV2">
-        <v>0</v>
-      </c>
-      <c r="AW2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>872</v>
       </c>
@@ -4143,43 +4137,46 @@
         <v>2</v>
       </c>
       <c r="AM3">
+        <v>66.730648916437048</v>
+      </c>
+      <c r="AN3">
+        <v>180.79488361545049</v>
+      </c>
+      <c r="AO3">
+        <v>41.464502875977445</v>
+      </c>
+      <c r="AP3">
+        <v>112.34073238254251</v>
+      </c>
+      <c r="AQ3">
+        <v>0.5</v>
+      </c>
+      <c r="AR3">
+        <v>0.3</v>
+      </c>
+      <c r="AS3">
+        <v>0.2</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>947</v>
+      </c>
+      <c r="AU3" t="s">
+        <v>947</v>
+      </c>
+      <c r="AV3" s="35">
+        <v>95000</v>
+      </c>
+      <c r="AW3">
+        <v>6</v>
+      </c>
+      <c r="AX3">
+        <v>1</v>
+      </c>
+      <c r="AY3">
         <v>3</v>
       </c>
-      <c r="AN3">
-        <v>2</v>
-      </c>
-      <c r="AO3">
-        <v>1</v>
-      </c>
-      <c r="AP3">
-        <v>66.730648916437048</v>
-      </c>
-      <c r="AQ3">
-        <v>180.79488361545049</v>
-      </c>
-      <c r="AR3">
-        <v>41.464502875977445</v>
-      </c>
-      <c r="AS3">
-        <v>112.34073238254251</v>
-      </c>
-      <c r="AT3">
-        <v>0.5</v>
-      </c>
-      <c r="AU3">
-        <v>0.3</v>
-      </c>
-      <c r="AV3">
-        <v>0.2</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>947</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>873</v>
       </c>
@@ -4295,43 +4292,46 @@
         <v>3</v>
       </c>
       <c r="AM4">
+        <v>54.000686345069504</v>
+      </c>
+      <c r="AN4">
+        <v>107.42790056424694</v>
+      </c>
+      <c r="AO4">
+        <v>33.554470855870157</v>
+      </c>
+      <c r="AP4">
+        <v>66.752602653159883</v>
+      </c>
+      <c r="AQ4">
+        <v>1</v>
+      </c>
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
+        <v>0</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>945</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>945</v>
+      </c>
+      <c r="AV4" s="35">
+        <v>650000</v>
+      </c>
+      <c r="AW4">
+        <v>3</v>
+      </c>
+      <c r="AX4">
+        <v>6</v>
+      </c>
+      <c r="AY4">
         <v>2</v>
       </c>
-      <c r="AN4">
-        <v>1</v>
-      </c>
-      <c r="AO4">
-        <v>3</v>
-      </c>
-      <c r="AP4">
-        <v>54.000686345069504</v>
-      </c>
-      <c r="AQ4">
-        <v>107.42790056424694</v>
-      </c>
-      <c r="AR4">
-        <v>33.554470855870157</v>
-      </c>
-      <c r="AS4">
-        <v>66.752602653159883</v>
-      </c>
-      <c r="AT4">
-        <v>1</v>
-      </c>
-      <c r="AU4">
-        <v>0</v>
-      </c>
-      <c r="AV4">
-        <v>0</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>945</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>874</v>
       </c>
@@ -4447,43 +4447,46 @@
         <v>2</v>
       </c>
       <c r="AM5">
-        <v>3</v>
+        <v>59.07183056002777</v>
       </c>
       <c r="AN5">
+        <v>62.670818674705536</v>
+      </c>
+      <c r="AO5">
+        <v>36.705533782726235</v>
+      </c>
+      <c r="AP5">
+        <v>38.941841318391553</v>
+      </c>
+      <c r="AQ5">
+        <v>0.45</v>
+      </c>
+      <c r="AR5">
+        <v>0.45</v>
+      </c>
+      <c r="AS5">
+        <v>0.1</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>946</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>946</v>
+      </c>
+      <c r="AV5" s="35">
+        <v>250000</v>
+      </c>
+      <c r="AW5">
         <v>2</v>
       </c>
-      <c r="AO5">
-        <v>1</v>
-      </c>
-      <c r="AP5">
-        <v>59.07183056002777</v>
-      </c>
-      <c r="AQ5">
-        <v>62.670818674705536</v>
-      </c>
-      <c r="AR5">
-        <v>36.705533782726235</v>
-      </c>
-      <c r="AS5">
-        <v>38.941841318391553</v>
-      </c>
-      <c r="AT5">
-        <v>0.45</v>
-      </c>
-      <c r="AU5">
-        <v>0.45</v>
-      </c>
-      <c r="AV5">
-        <v>0.1</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>946</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AX5">
+        <v>2</v>
+      </c>
+      <c r="AY5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>875</v>
       </c>
@@ -4599,43 +4602,46 @@
         <v>3</v>
       </c>
       <c r="AM6">
-        <v>1</v>
+        <v>61.132335382406808</v>
       </c>
       <c r="AN6">
+        <v>510.85624675116685</v>
+      </c>
+      <c r="AO6">
+        <v>37.985872120818676</v>
+      </c>
+      <c r="AP6">
+        <v>317.43135510566225</v>
+      </c>
+      <c r="AQ6">
+        <v>1</v>
+      </c>
+      <c r="AR6">
+        <v>0</v>
+      </c>
+      <c r="AS6">
+        <v>0</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>945</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>945</v>
+      </c>
+      <c r="AV6" s="35">
+        <v>203000</v>
+      </c>
+      <c r="AW6">
+        <v>0</v>
+      </c>
+      <c r="AX6">
         <v>2</v>
       </c>
-      <c r="AO6">
-        <v>3</v>
-      </c>
-      <c r="AP6">
-        <v>61.132335382406808</v>
-      </c>
-      <c r="AQ6">
-        <v>510.85624675116685</v>
-      </c>
-      <c r="AR6">
-        <v>37.985872120818676</v>
-      </c>
-      <c r="AS6">
-        <v>317.43135510566225</v>
-      </c>
-      <c r="AT6">
-        <v>1</v>
-      </c>
-      <c r="AU6">
-        <v>0</v>
-      </c>
-      <c r="AV6">
-        <v>0</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>945</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>876</v>
       </c>
@@ -4750,44 +4756,47 @@
       <c r="AL7">
         <v>3</v>
       </c>
-      <c r="AM7">
-        <v>2</v>
-      </c>
-      <c r="AN7">
-        <v>1</v>
-      </c>
-      <c r="AO7">
-        <v>3</v>
+      <c r="AM7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>201</v>
       </c>
       <c r="AP7" t="s">
         <v>201</v>
       </c>
-      <c r="AQ7" t="s">
-        <v>201</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>201</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>201</v>
-      </c>
-      <c r="AT7">
+      <c r="AQ7">
         <v>0.1</v>
       </c>
-      <c r="AU7">
-        <v>0</v>
-      </c>
-      <c r="AV7">
+      <c r="AR7">
+        <v>0</v>
+      </c>
+      <c r="AS7">
         <v>0.9</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AT7" t="s">
         <v>944</v>
       </c>
-      <c r="AX7" t="s">
+      <c r="AU7" t="s">
         <v>944</v>
       </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AV7" s="35">
+        <v>13500000</v>
+      </c>
+      <c r="AW7">
+        <v>63</v>
+      </c>
+      <c r="AX7">
+        <v>10</v>
+      </c>
+      <c r="AY7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>877</v>
       </c>
@@ -4903,43 +4912,46 @@
         <v>3</v>
       </c>
       <c r="AM8">
-        <v>2</v>
+        <v>42.020373634883299</v>
       </c>
       <c r="AN8">
-        <v>1</v>
+        <v>244.99066061451242</v>
       </c>
       <c r="AO8">
+        <v>26.110249663765671</v>
+      </c>
+      <c r="AP8">
+        <v>152.23013887305163</v>
+      </c>
+      <c r="AQ8">
+        <v>0.9</v>
+      </c>
+      <c r="AR8">
+        <v>0.1</v>
+      </c>
+      <c r="AS8">
+        <v>0</v>
+      </c>
+      <c r="AT8" t="s">
+        <v>943</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>943</v>
+      </c>
+      <c r="AV8" s="35">
+        <v>2000</v>
+      </c>
+      <c r="AW8">
+        <v>5</v>
+      </c>
+      <c r="AX8">
+        <v>1</v>
+      </c>
+      <c r="AY8">
         <v>3</v>
       </c>
-      <c r="AP8">
-        <v>42.020373634883299</v>
-      </c>
-      <c r="AQ8">
-        <v>244.99066061451242</v>
-      </c>
-      <c r="AR8">
-        <v>26.110249663765671</v>
-      </c>
-      <c r="AS8">
-        <v>152.23013887305163</v>
-      </c>
-      <c r="AT8">
-        <v>0.9</v>
-      </c>
-      <c r="AU8">
-        <v>0.1</v>
-      </c>
-      <c r="AV8">
-        <v>0</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>943</v>
-      </c>
-      <c r="AX8" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>878</v>
       </c>
@@ -5055,43 +5067,46 @@
         <v>3</v>
       </c>
       <c r="AM9">
-        <v>1</v>
+        <v>69.284801167278431</v>
       </c>
       <c r="AN9">
-        <v>2</v>
+        <v>217.13337565699663</v>
       </c>
       <c r="AO9">
-        <v>3</v>
+        <v>43.051579505238429</v>
       </c>
       <c r="AP9">
-        <v>69.284801167278431</v>
+        <v>134.9204245065049</v>
       </c>
       <c r="AQ9">
-        <v>217.13337565699663</v>
+        <v>0.5</v>
       </c>
       <c r="AR9">
-        <v>43.051579505238429</v>
+        <v>0.5</v>
       </c>
       <c r="AS9">
-        <v>134.9204245065049</v>
-      </c>
-      <c r="AT9">
-        <v>0.5</v>
-      </c>
-      <c r="AU9">
-        <v>0.5</v>
-      </c>
-      <c r="AV9">
-        <v>0</v>
-      </c>
-      <c r="AW9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT9" t="s">
         <v>942</v>
       </c>
-      <c r="AX9" t="s">
+      <c r="AU9" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AV9" s="35">
+        <v>700000</v>
+      </c>
+      <c r="AW9">
+        <v>8</v>
+      </c>
+      <c r="AX9">
+        <v>7</v>
+      </c>
+      <c r="AY9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>879</v>
       </c>
@@ -5206,44 +5221,41 @@
       <c r="AL10">
         <v>2</v>
       </c>
-      <c r="AM10">
-        <v>3</v>
-      </c>
-      <c r="AN10">
-        <v>2</v>
-      </c>
-      <c r="AO10">
-        <v>1</v>
+      <c r="AM10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO10" t="s">
+        <v>201</v>
       </c>
       <c r="AP10" t="s">
         <v>201</v>
       </c>
-      <c r="AQ10" t="s">
-        <v>201</v>
-      </c>
-      <c r="AR10" t="s">
-        <v>201</v>
-      </c>
-      <c r="AS10" t="s">
-        <v>201</v>
-      </c>
-      <c r="AT10">
+      <c r="AQ10">
         <v>0.1</v>
       </c>
-      <c r="AU10">
+      <c r="AR10">
         <v>0.45</v>
       </c>
-      <c r="AV10">
+      <c r="AS10">
         <v>0.45</v>
       </c>
-      <c r="AW10" t="s">
+      <c r="AT10" t="s">
         <v>940</v>
       </c>
-      <c r="AX10" t="s">
+      <c r="AU10" t="s">
         <v>940</v>
       </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AX10">
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>880</v>
       </c>
@@ -5359,43 +5371,46 @@
         <v>3</v>
       </c>
       <c r="AM11">
-        <v>2</v>
+        <v>49.269501231495838</v>
       </c>
       <c r="AN11">
-        <v>1</v>
+        <v>219.39060746351947</v>
       </c>
       <c r="AO11">
+        <v>30.614648721153365</v>
+      </c>
+      <c r="AP11">
+        <v>136.32300332528004</v>
+      </c>
+      <c r="AQ11">
+        <v>0.5</v>
+      </c>
+      <c r="AR11">
+        <v>0</v>
+      </c>
+      <c r="AS11">
+        <v>0.5</v>
+      </c>
+      <c r="AT11" t="s">
+        <v>938</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>938</v>
+      </c>
+      <c r="AV11" s="35">
+        <v>350000</v>
+      </c>
+      <c r="AW11">
+        <v>10</v>
+      </c>
+      <c r="AX11">
         <v>3</v>
       </c>
-      <c r="AP11">
-        <v>49.269501231495838</v>
-      </c>
-      <c r="AQ11">
-        <v>219.39060746351947</v>
-      </c>
-      <c r="AR11">
-        <v>30.614648721153365</v>
-      </c>
-      <c r="AS11">
-        <v>136.32300332528004</v>
-      </c>
-      <c r="AT11">
-        <v>0.5</v>
-      </c>
-      <c r="AU11">
-        <v>0</v>
-      </c>
-      <c r="AV11">
-        <v>0.5</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>938</v>
-      </c>
-      <c r="AX11" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>881</v>
       </c>
@@ -5511,43 +5526,40 @@
         <v>3</v>
       </c>
       <c r="AM12">
-        <v>2</v>
+        <v>102.89933989204253</v>
       </c>
       <c r="AN12">
-        <v>1</v>
+        <v>195.67903527505888</v>
       </c>
       <c r="AO12">
-        <v>3</v>
+        <v>63.938685509153132</v>
       </c>
       <c r="AP12">
-        <v>102.89933989204253</v>
+        <v>121.58931544471467</v>
       </c>
       <c r="AQ12">
-        <v>195.67903527505888</v>
+        <v>0</v>
       </c>
       <c r="AR12">
-        <v>63.938685509153132</v>
+        <v>0.5</v>
       </c>
       <c r="AS12">
-        <v>121.58931544471467</v>
-      </c>
-      <c r="AT12">
-        <v>0</v>
-      </c>
-      <c r="AU12">
         <v>0.5</v>
       </c>
-      <c r="AV12">
-        <v>0.5</v>
-      </c>
-      <c r="AW12" t="s">
+      <c r="AT12" t="s">
         <v>936</v>
       </c>
-      <c r="AX12" t="s">
+      <c r="AU12" t="s">
         <v>936</v>
       </c>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AX12">
+        <v>0</v>
+      </c>
+      <c r="AY12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>882</v>
       </c>
@@ -5662,41 +5674,44 @@
       <c r="AL13">
         <v>2</v>
       </c>
-      <c r="AM13">
-        <v>2</v>
-      </c>
-      <c r="AN13">
-        <v>1</v>
-      </c>
-      <c r="AO13">
-        <v>3</v>
+      <c r="AM13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AO13" t="s">
+        <v>201</v>
       </c>
       <c r="AP13" t="s">
         <v>201</v>
       </c>
-      <c r="AQ13" t="s">
-        <v>201</v>
-      </c>
-      <c r="AR13" t="s">
-        <v>201</v>
-      </c>
-      <c r="AS13" t="s">
-        <v>201</v>
-      </c>
-      <c r="AT13">
+      <c r="AQ13">
         <v>0.5</v>
       </c>
-      <c r="AU13">
+      <c r="AR13">
         <v>0.45</v>
       </c>
-      <c r="AV13">
+      <c r="AS13">
         <v>0.05</v>
       </c>
-      <c r="AW13" t="s">
+      <c r="AT13" t="s">
         <v>933</v>
       </c>
-      <c r="AX13" t="s">
+      <c r="AU13" t="s">
         <v>933</v>
+      </c>
+      <c r="AV13" s="35">
+        <v>650000</v>
+      </c>
+      <c r="AW13">
+        <v>4</v>
+      </c>
+      <c r="AX13">
+        <v>6</v>
+      </c>
+      <c r="AY13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6266,200 +6281,200 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="37" t="s">
         <v>870</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="36"/>
-      <c r="O15" s="36"/>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="36" t="s">
         <v>210</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+      <c r="P17" s="36"/>
+      <c r="Q17" s="36"/>
+      <c r="R17" s="36"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="30"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="36"/>
+      <c r="P20" s="36"/>
+      <c r="Q20" s="36"/>
+      <c r="R20" s="36"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="36"/>
+      <c r="R21" s="36"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="36"/>
+      <c r="P22" s="36"/>
+      <c r="Q22" s="36"/>
+      <c r="R22" s="36"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
+      <c r="P23" s="36"/>
+      <c r="Q23" s="36"/>
+      <c r="R23" s="36"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="36" t="s">
         <v>221</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M31" t="s">
-        <v>978</v>
+        <v>971</v>
       </c>
     </row>
   </sheetData>
@@ -16158,188 +16173,283 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2A3B86-5A46-4641-9702-EE1A057656B6}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>889</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>967</v>
+        <v>889</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>980</v>
+        <v>963</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>973</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>871</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>872</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>872</v>
+      </c>
+      <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="37">
+      <c r="D3" s="35">
         <v>95000</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>873</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="37">
-        <v>650000</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
       </c>
       <c r="E3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>873</v>
+      </c>
+      <c r="B4" t="s">
+        <v>873</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="35">
+        <v>650000</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>874</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>874</v>
+      </c>
+      <c r="C5" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="37">
+      <c r="D5" s="35">
         <v>250000</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>875</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="37">
-        <v>203000</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>875</v>
+      </c>
+      <c r="B6" t="s">
+        <v>875</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="35">
+        <v>203000</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>876</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
+        <v>876</v>
+      </c>
+      <c r="C7" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="37">
+      <c r="D7" s="35">
         <v>13500000</v>
       </c>
-      <c r="D6">
+      <c r="E7">
         <v>63</v>
       </c>
-      <c r="E6">
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>877</v>
+      </c>
+      <c r="B8" t="s">
+        <v>877</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="35">
+        <v>2000</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>878</v>
+      </c>
+      <c r="B9" t="s">
+        <v>878</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="35">
+        <v>700000</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>879</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>880</v>
+      </c>
+      <c r="B11" t="s">
+        <v>880</v>
+      </c>
+      <c r="C11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="35">
+        <v>350000</v>
+      </c>
+      <c r="E11">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>877</v>
-      </c>
-      <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="37">
-        <v>2000</v>
-      </c>
-      <c r="D7">
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
         <v>5</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>878</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="37">
-        <v>700000</v>
-      </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>880</v>
-      </c>
-      <c r="B9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="37">
-        <v>350000</v>
-      </c>
-      <c r="D9">
-        <v>10</v>
-      </c>
-      <c r="E9">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>881</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>882</v>
+      </c>
+      <c r="B13" t="s">
+        <v>882</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="35">
+        <v>650000</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>882</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="37">
-        <v>650000</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>6</v>
+      <c r="G13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -17908,7 +18018,7 @@
         <v>173</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>975</v>
+        <v>968</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final for 2/10 meeting with Emily
</commit_message>
<xml_diff>
--- a/Data/master.xlsx
+++ b/Data/master.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ta0jrg1\Documents\Projects\FoodHubs\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E678832D-4EC1-4D6B-989B-2489CFE9FA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CF87C6-404B-4882-8AE9-78BADD955051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7FA3B4B5-9D15-B84A-A7DB-0A68A34FD98B}"/>
   </bookViews>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2318" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2357" uniqueCount="989">
   <si>
     <t>Hub</t>
   </si>
@@ -3112,20 +3112,52 @@
   </si>
   <si>
     <t>Miles 150 to 200</t>
+  </si>
+  <si>
+    <t>Household_R</t>
+  </si>
+  <si>
+    <t>0 to 10 Percent</t>
+  </si>
+  <si>
+    <t>Exclusive</t>
+  </si>
+  <si>
+    <t>20 to 30 Percent</t>
+  </si>
+  <si>
+    <t>80 to 90 Percent</t>
+  </si>
+  <si>
+    <t>10 to 20 Percent</t>
+  </si>
+  <si>
+    <t>60 to 70 Percent</t>
+  </si>
+  <si>
+    <t>30 to 40 Percent</t>
+  </si>
+  <si>
+    <t>40 to 50 Percent</t>
+  </si>
+  <si>
+    <t>Institutions_R</t>
+  </si>
+  <si>
+    <t>Wholesale_R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -3341,13 +3373,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3663,10 +3695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D66AB6-4D2C-4516-876E-80F25D4C8C14}">
-  <dimension ref="A1:AY13"/>
+  <dimension ref="A1:BB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AR9" sqref="AR9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3691,36 +3723,38 @@
     <col min="18" max="18" width="11.625" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="10.375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="9.5" customWidth="1"/>
+    <col min="25" max="25" width="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.875" customWidth="1"/>
-    <col min="43" max="43" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.875" customWidth="1"/>
-    <col min="45" max="45" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.875" customWidth="1"/>
+    <col min="46" max="46" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.875" customWidth="1"/>
+    <col min="48" max="48" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="261" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" ht="261" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>889</v>
       </c>
@@ -3784,98 +3818,107 @@
       <c r="U1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="W1" s="19" t="s">
+      <c r="V1" t="s">
+        <v>978</v>
+      </c>
+      <c r="W1" t="s">
+        <v>987</v>
+      </c>
+      <c r="X1" t="s">
+        <v>988</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AD1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AE1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AF1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" s="21" t="s">
+      <c r="AG1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="20" t="s">
+      <c r="AH1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="AF1" s="20" t="s">
+      <c r="AI1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>963</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>964</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>965</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>953</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>954</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>955</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>941</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>940</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>939</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>967</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>938</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>968</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>185</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>186</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>187</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>960</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>961</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>871</v>
       </c>
@@ -3940,13 +3983,13 @@
         <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>201</v>
+        <v>980</v>
       </c>
       <c r="W2" t="s">
-        <v>201</v>
+        <v>979</v>
       </c>
       <c r="X2" t="s">
-        <v>201</v>
+        <v>979</v>
       </c>
       <c r="Y2" t="s">
         <v>201</v>
@@ -3981,50 +4024,59 @@
       <c r="AI2" t="s">
         <v>201</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM2">
         <v>3</v>
       </c>
-      <c r="AK2">
+      <c r="AN2">
         <v>3</v>
       </c>
-      <c r="AL2">
+      <c r="AO2">
         <v>2</v>
       </c>
-      <c r="AM2">
+      <c r="AP2">
         <v>177.06984362075525</v>
       </c>
-      <c r="AN2">
+      <c r="AQ2">
         <v>502.86279698478472</v>
       </c>
-      <c r="AO2">
+      <c r="AR2">
         <v>110.02609983990698</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AS2" t="s">
         <v>970</v>
       </c>
-      <c r="AQ2">
+      <c r="AT2">
         <v>312.46445569423616</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AU2" t="s">
         <v>975</v>
       </c>
-      <c r="AS2" s="38">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="38">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="38">
-        <v>0</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AV2" s="36">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="36">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="36">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>872</v>
       </c>
@@ -4088,98 +4140,107 @@
       <c r="U3">
         <v>0</v>
       </c>
-      <c r="V3">
+      <c r="V3" t="s">
+        <v>979</v>
+      </c>
+      <c r="W3" t="s">
+        <v>982</v>
+      </c>
+      <c r="X3" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y3">
         <v>2</v>
       </c>
-      <c r="W3">
+      <c r="Z3">
         <v>3</v>
-      </c>
-      <c r="X3">
-        <v>3</v>
-      </c>
-      <c r="Y3">
-        <v>3</v>
-      </c>
-      <c r="Z3">
-        <v>2</v>
       </c>
       <c r="AA3">
         <v>3</v>
       </c>
       <c r="AB3">
+        <v>3</v>
+      </c>
+      <c r="AC3">
         <v>2</v>
-      </c>
-      <c r="AC3">
-        <v>3</v>
       </c>
       <c r="AD3">
         <v>3</v>
       </c>
       <c r="AE3">
+        <v>2</v>
+      </c>
+      <c r="AF3">
         <v>3</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
+        <v>3</v>
+      </c>
+      <c r="AH3">
+        <v>3</v>
+      </c>
+      <c r="AI3">
         <v>2</v>
       </c>
-      <c r="AG3">
+      <c r="AJ3">
         <v>2.6</v>
       </c>
-      <c r="AH3">
+      <c r="AK3">
         <v>2.75</v>
       </c>
-      <c r="AI3">
+      <c r="AL3">
         <v>2.5</v>
       </c>
-      <c r="AJ3">
+      <c r="AM3">
         <v>3</v>
       </c>
-      <c r="AK3">
+      <c r="AN3">
         <v>3</v>
       </c>
-      <c r="AL3">
+      <c r="AO3">
         <v>2</v>
       </c>
-      <c r="AM3">
+      <c r="AP3">
         <v>66.730648916437048</v>
       </c>
-      <c r="AN3">
+      <c r="AQ3">
         <v>180.79488361545049</v>
       </c>
-      <c r="AO3">
+      <c r="AR3">
         <v>41.464502875977445</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AS3" t="s">
         <v>971</v>
       </c>
-      <c r="AQ3">
+      <c r="AT3">
         <v>112.34073238254251</v>
       </c>
-      <c r="AR3" t="s">
+      <c r="AU3" t="s">
         <v>976</v>
       </c>
-      <c r="AS3" s="38">
+      <c r="AV3" s="36">
         <v>0.5</v>
       </c>
-      <c r="AT3" s="38">
+      <c r="AW3" s="36">
         <v>0.3</v>
       </c>
-      <c r="AU3" s="38">
+      <c r="AX3" s="36">
         <v>0.2</v>
       </c>
-      <c r="AV3" s="35">
+      <c r="AY3" s="35">
         <v>95000</v>
       </c>
-      <c r="AW3">
+      <c r="AZ3">
         <v>6</v>
       </c>
-      <c r="AX3">
-        <v>1</v>
-      </c>
-      <c r="AY3">
+      <c r="BA3">
+        <v>1</v>
+      </c>
+      <c r="BB3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>873</v>
       </c>
@@ -4243,17 +4304,17 @@
       <c r="U4">
         <v>0</v>
       </c>
-      <c r="V4">
+      <c r="V4" t="s">
+        <v>979</v>
+      </c>
+      <c r="W4" t="s">
+        <v>980</v>
+      </c>
+      <c r="X4" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y4">
         <v>2</v>
-      </c>
-      <c r="W4">
-        <v>3</v>
-      </c>
-      <c r="X4">
-        <v>3</v>
-      </c>
-      <c r="Y4">
-        <v>3</v>
       </c>
       <c r="Z4">
         <v>3</v>
@@ -4262,79 +4323,88 @@
         <v>3</v>
       </c>
       <c r="AB4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD4">
         <v>3</v>
       </c>
       <c r="AE4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF4">
         <v>2</v>
       </c>
       <c r="AG4">
+        <v>3</v>
+      </c>
+      <c r="AH4">
+        <v>3</v>
+      </c>
+      <c r="AI4">
+        <v>2</v>
+      </c>
+      <c r="AJ4">
         <v>2.8</v>
       </c>
-      <c r="AH4">
+      <c r="AK4">
         <v>2.5</v>
       </c>
-      <c r="AI4">
+      <c r="AL4">
         <v>2.5</v>
       </c>
-      <c r="AJ4">
+      <c r="AM4">
         <v>2</v>
       </c>
-      <c r="AK4">
+      <c r="AN4">
         <v>2</v>
       </c>
-      <c r="AL4">
+      <c r="AO4">
         <v>3</v>
       </c>
-      <c r="AM4">
+      <c r="AP4">
         <v>54.000686345069504</v>
       </c>
-      <c r="AN4">
+      <c r="AQ4">
         <v>107.42790056424694</v>
       </c>
-      <c r="AO4">
+      <c r="AR4">
         <v>33.554470855870157</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="AS4" t="s">
         <v>972</v>
       </c>
-      <c r="AQ4">
+      <c r="AT4">
         <v>66.752602653159883</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="AU4" t="s">
         <v>969</v>
       </c>
-      <c r="AS4" s="38">
-        <v>1</v>
-      </c>
-      <c r="AT4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AU4" s="38">
-        <v>0</v>
-      </c>
-      <c r="AV4" s="35">
+      <c r="AV4" s="36">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="36">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="35">
         <v>650000</v>
       </c>
-      <c r="AW4">
+      <c r="AZ4">
         <v>3</v>
       </c>
-      <c r="AX4">
+      <c r="BA4">
         <v>6</v>
       </c>
-      <c r="AY4">
+      <c r="BB4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>874</v>
       </c>
@@ -4398,98 +4468,107 @@
       <c r="U5">
         <v>3</v>
       </c>
-      <c r="V5">
+      <c r="V5" t="s">
+        <v>979</v>
+      </c>
+      <c r="W5" t="s">
+        <v>984</v>
+      </c>
+      <c r="X5" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y5">
         <v>2</v>
       </c>
-      <c r="W5">
+      <c r="Z5">
         <v>3</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>3</v>
       </c>
-      <c r="Y5">
-        <v>1</v>
-      </c>
-      <c r="Z5">
-        <v>1</v>
-      </c>
-      <c r="AA5">
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
         <v>2</v>
       </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-      <c r="AC5">
-        <v>1</v>
-      </c>
-      <c r="AD5">
-        <v>1</v>
-      </c>
       <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
         <v>2</v>
       </c>
-      <c r="AF5">
-        <v>1</v>
-      </c>
-      <c r="AG5">
-        <v>2</v>
-      </c>
-      <c r="AH5">
-        <v>1.25</v>
-      </c>
       <c r="AI5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="AJ5">
         <v>2</v>
       </c>
       <c r="AK5">
+        <v>1.25</v>
+      </c>
+      <c r="AL5">
+        <v>1.5</v>
+      </c>
+      <c r="AM5">
         <v>2</v>
       </c>
-      <c r="AL5">
+      <c r="AN5">
         <v>2</v>
       </c>
-      <c r="AM5">
+      <c r="AO5">
+        <v>2</v>
+      </c>
+      <c r="AP5">
         <v>59.07183056002777</v>
       </c>
-      <c r="AN5">
+      <c r="AQ5">
         <v>62.670818674705536</v>
       </c>
-      <c r="AO5">
+      <c r="AR5">
         <v>36.705533782726235</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AS5" t="s">
         <v>972</v>
       </c>
-      <c r="AQ5">
+      <c r="AT5">
         <v>38.941841318391553</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AU5" t="s">
         <v>969</v>
       </c>
-      <c r="AS5" s="38">
+      <c r="AV5" s="36">
         <v>0.45</v>
       </c>
-      <c r="AT5" s="38">
+      <c r="AW5" s="36">
         <v>0.45</v>
       </c>
-      <c r="AU5" s="38">
+      <c r="AX5" s="36">
         <v>0.1</v>
       </c>
-      <c r="AV5" s="35">
+      <c r="AY5" s="35">
         <v>250000</v>
       </c>
-      <c r="AW5">
+      <c r="AZ5">
         <v>2</v>
       </c>
-      <c r="AX5">
+      <c r="BA5">
         <v>2</v>
       </c>
-      <c r="AY5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="BB5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>875</v>
       </c>
@@ -4553,17 +4632,17 @@
       <c r="U6">
         <v>0</v>
       </c>
-      <c r="V6">
+      <c r="V6" t="s">
+        <v>982</v>
+      </c>
+      <c r="W6" t="s">
+        <v>981</v>
+      </c>
+      <c r="X6" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y6">
         <v>2</v>
-      </c>
-      <c r="W6">
-        <v>3</v>
-      </c>
-      <c r="X6">
-        <v>3</v>
-      </c>
-      <c r="Y6">
-        <v>3</v>
       </c>
       <c r="Z6">
         <v>3</v>
@@ -4587,7 +4666,7 @@
         <v>3</v>
       </c>
       <c r="AG6">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="AH6">
         <v>3</v>
@@ -4596,55 +4675,64 @@
         <v>3</v>
       </c>
       <c r="AJ6">
-        <v>2</v>
+        <v>2.8</v>
       </c>
       <c r="AK6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL6">
         <v>3</v>
       </c>
       <c r="AM6">
+        <v>2</v>
+      </c>
+      <c r="AN6">
+        <v>2</v>
+      </c>
+      <c r="AO6">
+        <v>3</v>
+      </c>
+      <c r="AP6">
         <v>61.132335382406808</v>
       </c>
-      <c r="AN6">
+      <c r="AQ6">
         <v>510.85624675116685</v>
       </c>
-      <c r="AO6">
+      <c r="AR6">
         <v>37.985872120818676</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AS6" t="s">
         <v>972</v>
       </c>
-      <c r="AQ6">
+      <c r="AT6">
         <v>317.43135510566225</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AU6" t="s">
         <v>975</v>
       </c>
-      <c r="AS6" s="38">
-        <v>1</v>
-      </c>
-      <c r="AT6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AU6" s="38">
-        <v>0</v>
-      </c>
-      <c r="AV6" s="35">
+      <c r="AV6" s="36">
+        <v>1</v>
+      </c>
+      <c r="AW6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="36">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="35">
         <v>203000</v>
       </c>
-      <c r="AW6">
-        <v>0</v>
-      </c>
-      <c r="AX6">
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6">
         <v>2</v>
       </c>
-      <c r="AY6">
+      <c r="BB6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>876</v>
       </c>
@@ -4709,13 +4797,13 @@
         <v>0</v>
       </c>
       <c r="V7" t="s">
-        <v>201</v>
+        <v>979</v>
       </c>
       <c r="W7" t="s">
-        <v>201</v>
+        <v>979</v>
       </c>
       <c r="X7" t="s">
-        <v>201</v>
+        <v>979</v>
       </c>
       <c r="Y7" t="s">
         <v>201</v>
@@ -4750,23 +4838,23 @@
       <c r="AI7" t="s">
         <v>201</v>
       </c>
-      <c r="AJ7">
+      <c r="AJ7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM7">
         <v>2</v>
       </c>
-      <c r="AK7">
+      <c r="AN7">
         <v>2</v>
       </c>
-      <c r="AL7">
+      <c r="AO7">
         <v>3</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>201</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>201</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>201</v>
       </c>
       <c r="AP7" t="s">
         <v>201</v>
@@ -4777,29 +4865,38 @@
       <c r="AR7" t="s">
         <v>201</v>
       </c>
-      <c r="AS7" s="38">
+      <c r="AS7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AV7" s="36">
         <v>0.1</v>
       </c>
-      <c r="AT7" s="38">
-        <v>0</v>
-      </c>
-      <c r="AU7" s="38">
+      <c r="AW7" s="36">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="36">
         <v>0.9</v>
       </c>
-      <c r="AV7" s="35">
+      <c r="AY7" s="35">
         <v>13500000</v>
       </c>
-      <c r="AW7">
+      <c r="AZ7">
         <v>63</v>
       </c>
-      <c r="AX7">
+      <c r="BA7">
         <v>10</v>
       </c>
-      <c r="AY7">
+      <c r="BB7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>877</v>
       </c>
@@ -4863,98 +4960,107 @@
       <c r="U8">
         <v>5</v>
       </c>
-      <c r="V8">
+      <c r="V8" t="s">
+        <v>982</v>
+      </c>
+      <c r="W8" t="s">
+        <v>983</v>
+      </c>
+      <c r="X8" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y8">
         <v>2</v>
-      </c>
-      <c r="W8">
-        <v>3</v>
-      </c>
-      <c r="X8">
-        <v>3</v>
-      </c>
-      <c r="Y8">
-        <v>3</v>
       </c>
       <c r="Z8">
         <v>3</v>
       </c>
       <c r="AA8">
+        <v>3</v>
+      </c>
+      <c r="AB8">
+        <v>3</v>
+      </c>
+      <c r="AC8">
+        <v>3</v>
+      </c>
+      <c r="AD8">
         <v>2</v>
-      </c>
-      <c r="AB8">
-        <v>2</v>
-      </c>
-      <c r="AC8">
-        <v>2</v>
-      </c>
-      <c r="AD8">
-        <v>3</v>
       </c>
       <c r="AE8">
         <v>2</v>
       </c>
       <c r="AF8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG8">
+        <v>3</v>
+      </c>
+      <c r="AH8">
+        <v>2</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
         <v>2.8</v>
       </c>
-      <c r="AH8">
+      <c r="AK8">
         <v>2.25</v>
       </c>
-      <c r="AI8">
+      <c r="AL8">
         <v>1.5</v>
       </c>
-      <c r="AJ8">
+      <c r="AM8">
         <v>2</v>
       </c>
-      <c r="AK8">
-        <v>1</v>
-      </c>
-      <c r="AL8">
+      <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
         <v>3</v>
       </c>
-      <c r="AM8">
+      <c r="AP8">
         <v>42.020373634883299</v>
       </c>
-      <c r="AN8">
+      <c r="AQ8">
         <v>244.99066061451242</v>
       </c>
-      <c r="AO8">
+      <c r="AR8">
         <v>26.110249663765671</v>
       </c>
-      <c r="AP8" t="s">
+      <c r="AS8" t="s">
         <v>973</v>
       </c>
-      <c r="AQ8">
+      <c r="AT8">
         <v>152.23013887305163</v>
       </c>
-      <c r="AR8" t="s">
+      <c r="AU8" t="s">
         <v>977</v>
       </c>
-      <c r="AS8" s="38">
+      <c r="AV8" s="36">
         <v>0.9</v>
       </c>
-      <c r="AT8" s="38">
+      <c r="AW8" s="36">
         <v>0.1</v>
       </c>
-      <c r="AU8" s="38">
-        <v>0</v>
-      </c>
-      <c r="AV8" s="35">
+      <c r="AX8" s="36">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="35">
         <v>2000</v>
       </c>
-      <c r="AW8">
+      <c r="AZ8">
         <v>5</v>
       </c>
-      <c r="AX8">
-        <v>1</v>
-      </c>
-      <c r="AY8">
+      <c r="BA8">
+        <v>1</v>
+      </c>
+      <c r="BB8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>878</v>
       </c>
@@ -5018,23 +5124,23 @@
       <c r="U9">
         <v>0</v>
       </c>
-      <c r="V9">
+      <c r="V9" t="s">
+        <v>982</v>
+      </c>
+      <c r="W9" t="s">
+        <v>983</v>
+      </c>
+      <c r="X9" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y9">
         <v>3</v>
       </c>
-      <c r="W9">
+      <c r="Z9">
         <v>3</v>
       </c>
-      <c r="X9">
+      <c r="AA9">
         <v>3</v>
-      </c>
-      <c r="Y9">
-        <v>2</v>
-      </c>
-      <c r="Z9">
-        <v>2</v>
-      </c>
-      <c r="AA9">
-        <v>2</v>
       </c>
       <c r="AB9">
         <v>2</v>
@@ -5052,7 +5158,7 @@
         <v>2</v>
       </c>
       <c r="AG9">
-        <v>2.6</v>
+        <v>2</v>
       </c>
       <c r="AH9">
         <v>2</v>
@@ -5061,55 +5167,64 @@
         <v>2</v>
       </c>
       <c r="AJ9">
+        <v>2.6</v>
+      </c>
+      <c r="AK9">
+        <v>2</v>
+      </c>
+      <c r="AL9">
+        <v>2</v>
+      </c>
+      <c r="AM9">
         <v>2.5</v>
       </c>
-      <c r="AK9">
+      <c r="AN9">
         <v>3</v>
       </c>
-      <c r="AL9">
+      <c r="AO9">
         <v>3</v>
       </c>
-      <c r="AM9">
+      <c r="AP9">
         <v>69.284801167278431</v>
       </c>
-      <c r="AN9">
+      <c r="AQ9">
         <v>217.13337565699663</v>
       </c>
-      <c r="AO9">
+      <c r="AR9">
         <v>43.051579505238429</v>
       </c>
-      <c r="AP9" t="s">
+      <c r="AS9" t="s">
         <v>971</v>
       </c>
-      <c r="AQ9">
+      <c r="AT9">
         <v>134.9204245065049</v>
       </c>
-      <c r="AR9" t="s">
+      <c r="AU9" t="s">
         <v>976</v>
       </c>
-      <c r="AS9" s="38">
+      <c r="AV9" s="36">
         <v>0.5</v>
       </c>
-      <c r="AT9" s="38">
+      <c r="AW9" s="36">
         <v>0.5</v>
       </c>
-      <c r="AU9" s="38">
-        <v>0</v>
-      </c>
-      <c r="AV9" s="35">
+      <c r="AX9" s="36">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="35">
         <v>700000</v>
       </c>
-      <c r="AW9">
+      <c r="AZ9">
         <v>8</v>
       </c>
-      <c r="AX9">
+      <c r="BA9">
         <v>7</v>
       </c>
-      <c r="AY9">
+      <c r="BB9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>879</v>
       </c>
@@ -5174,13 +5289,13 @@
         <v>33</v>
       </c>
       <c r="V10" t="s">
-        <v>201</v>
+        <v>981</v>
       </c>
       <c r="W10" t="s">
-        <v>201</v>
+        <v>985</v>
       </c>
       <c r="X10" t="s">
-        <v>201</v>
+        <v>981</v>
       </c>
       <c r="Y10" t="s">
         <v>201</v>
@@ -5215,23 +5330,23 @@
       <c r="AI10" t="s">
         <v>201</v>
       </c>
-      <c r="AJ10">
+      <c r="AJ10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM10">
         <v>3</v>
       </c>
-      <c r="AK10">
+      <c r="AN10">
         <v>3</v>
       </c>
-      <c r="AL10">
+      <c r="AO10">
         <v>2</v>
-      </c>
-      <c r="AM10" t="s">
-        <v>201</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>201</v>
-      </c>
-      <c r="AO10" t="s">
-        <v>201</v>
       </c>
       <c r="AP10" t="s">
         <v>201</v>
@@ -5242,23 +5357,32 @@
       <c r="AR10" t="s">
         <v>201</v>
       </c>
-      <c r="AS10" s="38">
+      <c r="AS10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AV10" s="36">
         <v>0.1</v>
       </c>
-      <c r="AT10" s="38">
+      <c r="AW10" s="36">
         <v>0.45</v>
       </c>
-      <c r="AU10" s="38">
+      <c r="AX10" s="36">
         <v>0.45</v>
       </c>
-      <c r="AX10">
-        <v>0</v>
-      </c>
-      <c r="AY10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="BA10">
+        <v>0</v>
+      </c>
+      <c r="BB10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>880</v>
       </c>
@@ -5322,17 +5446,17 @@
       <c r="U11">
         <v>28</v>
       </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
-      <c r="W11">
-        <v>3</v>
-      </c>
-      <c r="X11">
-        <v>3</v>
+      <c r="V11" t="s">
+        <v>981</v>
+      </c>
+      <c r="W11" t="s">
+        <v>986</v>
+      </c>
+      <c r="X11" t="s">
+        <v>981</v>
       </c>
       <c r="Y11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z11">
         <v>3</v>
@@ -5344,76 +5468,85 @@
         <v>3</v>
       </c>
       <c r="AC11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD11">
         <v>3</v>
       </c>
       <c r="AE11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF11">
         <v>2</v>
       </c>
       <c r="AG11">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="AH11">
-        <v>2.75</v>
+        <v>2</v>
       </c>
       <c r="AI11">
         <v>2</v>
       </c>
       <c r="AJ11">
+        <v>2.6</v>
+      </c>
+      <c r="AK11">
+        <v>2.75</v>
+      </c>
+      <c r="AL11">
         <v>2</v>
       </c>
-      <c r="AK11">
+      <c r="AM11">
         <v>2</v>
       </c>
-      <c r="AL11">
+      <c r="AN11">
+        <v>2</v>
+      </c>
+      <c r="AO11">
         <v>3</v>
       </c>
-      <c r="AM11">
+      <c r="AP11">
         <v>49.269501231495838</v>
       </c>
-      <c r="AN11">
+      <c r="AQ11">
         <v>219.39060746351947</v>
       </c>
-      <c r="AO11">
+      <c r="AR11">
         <v>30.614648721153365</v>
       </c>
-      <c r="AP11" t="s">
+      <c r="AS11" t="s">
         <v>972</v>
       </c>
-      <c r="AQ11">
+      <c r="AT11">
         <v>136.32300332528004</v>
       </c>
-      <c r="AR11" t="s">
+      <c r="AU11" t="s">
         <v>976</v>
       </c>
-      <c r="AS11" s="38">
+      <c r="AV11" s="36">
         <v>0.5</v>
       </c>
-      <c r="AT11" s="38">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="38">
+      <c r="AW11" s="36">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="36">
         <v>0.5</v>
       </c>
-      <c r="AV11" s="35">
+      <c r="AY11" s="35">
         <v>350000</v>
       </c>
-      <c r="AW11">
+      <c r="AZ11">
         <v>10</v>
       </c>
-      <c r="AX11">
+      <c r="BA11">
         <v>3</v>
       </c>
-      <c r="AY11">
+      <c r="BB11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>881</v>
       </c>
@@ -5478,13 +5611,13 @@
         <v>90</v>
       </c>
       <c r="V12" t="s">
-        <v>201</v>
+        <v>979</v>
       </c>
       <c r="W12" t="s">
-        <v>201</v>
+        <v>983</v>
       </c>
       <c r="X12" t="s">
-        <v>201</v>
+        <v>982</v>
       </c>
       <c r="Y12" t="s">
         <v>201</v>
@@ -5519,50 +5652,59 @@
       <c r="AI12" t="s">
         <v>201</v>
       </c>
-      <c r="AJ12">
+      <c r="AJ12" t="s">
+        <v>201</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>201</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM12">
         <v>2</v>
       </c>
-      <c r="AK12">
+      <c r="AN12">
         <v>2</v>
       </c>
-      <c r="AL12">
+      <c r="AO12">
         <v>3</v>
       </c>
-      <c r="AM12">
+      <c r="AP12">
         <v>102.89933989204253</v>
       </c>
-      <c r="AN12">
+      <c r="AQ12">
         <v>195.67903527505888</v>
       </c>
-      <c r="AO12">
+      <c r="AR12">
         <v>63.938685509153132</v>
       </c>
-      <c r="AP12" t="s">
+      <c r="AS12" t="s">
         <v>974</v>
       </c>
-      <c r="AQ12">
+      <c r="AT12">
         <v>121.58931544471467</v>
       </c>
-      <c r="AR12" t="s">
+      <c r="AU12" t="s">
         <v>976</v>
       </c>
-      <c r="AS12" s="38">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="38">
+      <c r="AV12" s="36">
+        <v>0</v>
+      </c>
+      <c r="AW12" s="36">
         <v>0.5</v>
       </c>
-      <c r="AU12" s="38">
+      <c r="AX12" s="36">
         <v>0.5</v>
       </c>
-      <c r="AX12">
-        <v>0</v>
-      </c>
-      <c r="AY12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="BA12">
+        <v>0</v>
+      </c>
+      <c r="BB12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>882</v>
       </c>
@@ -5626,65 +5768,65 @@
       <c r="U13">
         <v>0</v>
       </c>
-      <c r="V13">
+      <c r="V13" t="s">
+        <v>982</v>
+      </c>
+      <c r="W13" t="s">
+        <v>981</v>
+      </c>
+      <c r="X13" t="s">
+        <v>979</v>
+      </c>
+      <c r="Y13">
         <v>3</v>
       </c>
-      <c r="W13">
+      <c r="Z13">
         <v>3</v>
-      </c>
-      <c r="X13">
-        <v>3</v>
-      </c>
-      <c r="Y13">
-        <v>1</v>
-      </c>
-      <c r="Z13">
-        <v>1</v>
       </c>
       <c r="AA13">
         <v>3</v>
       </c>
       <c r="AB13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD13">
         <v>3</v>
       </c>
       <c r="AE13">
+        <v>0</v>
+      </c>
+      <c r="AF13">
         <v>2</v>
       </c>
-      <c r="AF13">
-        <v>1</v>
-      </c>
       <c r="AG13">
+        <v>3</v>
+      </c>
+      <c r="AH13">
+        <v>2</v>
+      </c>
+      <c r="AI13">
+        <v>1</v>
+      </c>
+      <c r="AJ13">
         <v>2.2000000000000002</v>
       </c>
-      <c r="AH13">
+      <c r="AK13">
         <v>2.6666666666666665</v>
       </c>
-      <c r="AI13">
+      <c r="AL13">
         <v>1.5</v>
       </c>
-      <c r="AJ13">
+      <c r="AM13">
         <v>2</v>
       </c>
-      <c r="AK13">
+      <c r="AN13">
         <v>2</v>
       </c>
-      <c r="AL13">
+      <c r="AO13">
         <v>2</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>201</v>
-      </c>
-      <c r="AN13" t="s">
-        <v>201</v>
-      </c>
-      <c r="AO13" t="s">
-        <v>201</v>
       </c>
       <c r="AP13" t="s">
         <v>201</v>
@@ -5695,25 +5837,34 @@
       <c r="AR13" t="s">
         <v>201</v>
       </c>
-      <c r="AS13" s="38">
+      <c r="AS13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AV13" s="36">
         <v>0.5</v>
       </c>
-      <c r="AT13" s="38">
+      <c r="AW13" s="36">
         <v>0.45</v>
       </c>
-      <c r="AU13" s="38">
+      <c r="AX13" s="36">
         <v>0.05</v>
       </c>
-      <c r="AV13" s="35">
+      <c r="AY13" s="35">
         <v>650000</v>
       </c>
-      <c r="AW13">
+      <c r="AZ13">
         <v>4</v>
       </c>
-      <c r="AX13">
+      <c r="BA13">
         <v>6</v>
       </c>
-      <c r="AY13">
+      <c r="BB13">
         <v>2</v>
       </c>
     </row>
@@ -6284,196 +6435,196 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="38" t="s">
         <v>870</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="36"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="36"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="36"/>
-      <c r="R16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
-      <c r="K17" s="36"/>
-      <c r="L17" s="36"/>
-      <c r="M17" s="36"/>
-      <c r="N17" s="36"/>
-      <c r="O17" s="36"/>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="36"/>
-      <c r="R17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="30"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="36"/>
-      <c r="O20" s="36"/>
-      <c r="P20" s="36"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37"/>
+      <c r="O20" s="37"/>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="37"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
-      <c r="Q21" s="36"/>
-      <c r="R21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="37"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
-      <c r="P23" s="36"/>
-      <c r="Q23" s="36"/>
-      <c r="R23" s="36"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="37"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M31" t="s">

</xml_diff>